<commit_message>
made it easier to train models and predict code
</commit_message>
<xml_diff>
--- a/predicted_trajectories_combined.xlsx
+++ b/predicted_trajectories_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TdrDi\Documents\GitHub\Badmintobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B778421D-A477-48E2-93FC-4DE8520C97B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C36C52-0051-47E1-8AB7-27D2D2AA73B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,13 +415,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1458.28853671407</v>
+        <v>1487.511676915803</v>
       </c>
       <c r="C2">
         <v>75.30677895524029</v>
       </c>
       <c r="D2">
-        <v>2082.5783986273941</v>
+        <v>1883.468544629751</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -429,13 +429,13 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="B3">
-        <v>2401.708228290338</v>
+        <v>2597.1443555309761</v>
       </c>
       <c r="C3">
         <v>787.92953529326223</v>
       </c>
       <c r="D3">
-        <v>2750.2063014361029</v>
+        <v>2631.0266361136132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -443,13 +443,13 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="B4">
-        <v>3266.985741789576</v>
+        <v>3749.2276811183551</v>
       </c>
       <c r="C4">
         <v>629.69371985358066</v>
       </c>
       <c r="D4">
-        <v>3331.7896158004828</v>
+        <v>3361.049035746008</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -457,13 +457,13 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <v>3750.7040811082229</v>
+        <v>4359.7024365325342</v>
       </c>
       <c r="C5">
         <v>758.97585213288357</v>
       </c>
       <c r="D5">
-        <v>3675.7703735235441</v>
+        <v>3702.6385577445481</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -471,13 +471,13 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6">
-        <v>4116.455524407289</v>
+        <v>4867.7790804145307</v>
       </c>
       <c r="C6">
         <v>917.37983237113633</v>
       </c>
       <c r="D6">
-        <v>3893.1397581281012</v>
+        <v>3936.7122999905491</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -485,13 +485,13 @@
         <v>0.16666666666666671</v>
       </c>
       <c r="B7">
-        <v>4304.1172750126862</v>
+        <v>5477.0020110422483</v>
       </c>
       <c r="C7">
         <v>797.83541499781472</v>
       </c>
       <c r="D7">
-        <v>4032.3837177528289</v>
+        <v>4019.2463258656821</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -499,13 +499,13 @@
         <v>0.2</v>
       </c>
       <c r="B8">
-        <v>4637.7329269030261</v>
+        <v>5870.9757057273737</v>
       </c>
       <c r="C8">
         <v>612.48294812243864</v>
       </c>
       <c r="D8">
-        <v>4071.4539642214372</v>
+        <v>4056.8255077806839</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -513,13 +513,13 @@
         <v>0.23333333333333331</v>
       </c>
       <c r="B9">
-        <v>4930.6467487052932</v>
+        <v>6108.2672100881236</v>
       </c>
       <c r="C9">
         <v>713.9465289679988</v>
       </c>
       <c r="D9">
-        <v>4077.0091807035369</v>
+        <v>4019.119389661651</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -527,13 +527,13 @@
         <v>0.26666666666666672</v>
       </c>
       <c r="B10">
-        <v>5275.3020121830314</v>
+        <v>6509.2126481888808</v>
       </c>
       <c r="C10">
         <v>768.78690065357648</v>
       </c>
       <c r="D10">
-        <v>3958.733767256942</v>
+        <v>3938.0230635159801</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -541,13 +541,13 @@
         <v>0.3</v>
       </c>
       <c r="B11">
-        <v>5353.3748653588764</v>
+        <v>6656.6219839515343</v>
       </c>
       <c r="C11">
         <v>786.71056401306043</v>
       </c>
       <c r="D11">
-        <v>3909.1793259317942</v>
+        <v>3898.0037236374642</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -555,13 +555,13 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B12">
-        <v>5507.0408650933296</v>
+        <v>6830.4194273670109</v>
       </c>
       <c r="C12">
         <v>801.40533568136664</v>
       </c>
       <c r="D12">
-        <v>3806.2562820921598</v>
+        <v>3764.5337586066212</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -569,13 +569,13 @@
         <v>0.36666666666666659</v>
       </c>
       <c r="B13">
-        <v>6029.2278668691724</v>
+        <v>7114.3915848310071</v>
       </c>
       <c r="C13">
         <v>876.08553291692965</v>
       </c>
       <c r="D13">
-        <v>3514.021756200269</v>
+        <v>3530.0264109258378</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -583,13 +583,13 @@
         <v>0.4</v>
       </c>
       <c r="B14">
-        <v>5765.3611224777324</v>
+        <v>7253.2620127701339</v>
       </c>
       <c r="C14">
         <v>948.6324758754879</v>
       </c>
       <c r="D14">
-        <v>3432.8005114011712</v>
+        <v>3308.580783525048</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -597,13 +597,13 @@
         <v>0.43333333333333329</v>
       </c>
       <c r="B15">
-        <v>5840.0746989451036</v>
+        <v>7389.2408480578224</v>
       </c>
       <c r="C15">
         <v>1046.6860549086171</v>
       </c>
       <c r="D15">
-        <v>3116.4050221711941</v>
+        <v>3141.431113705878</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -611,13 +611,13 @@
         <v>0.46666666666666667</v>
       </c>
       <c r="B16">
-        <v>5979.8395295733317</v>
+        <v>7599.0573863269792</v>
       </c>
       <c r="C16">
         <v>1036.2871006804739</v>
       </c>
       <c r="D16">
-        <v>2822.5255673532338</v>
+        <v>2867.4796875735278</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -625,13 +625,13 @@
         <v>0.5</v>
       </c>
       <c r="B17">
-        <v>6032.0791187281784</v>
+        <v>7726.4113143407349</v>
       </c>
       <c r="C17">
         <v>1080.498104115301</v>
       </c>
       <c r="D17">
-        <v>2512.4540502214682</v>
+        <v>2554.1921565376101</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -639,13 +639,13 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="B18">
-        <v>6109.6789040524081</v>
+        <v>7847.7566768792394</v>
       </c>
       <c r="C18">
         <v>1048.9810449928791</v>
       </c>
       <c r="D18">
-        <v>2170.947263601804</v>
+        <v>2191.9683281496891</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -653,13 +653,13 @@
         <v>0.56666666666666665</v>
       </c>
       <c r="B19">
-        <v>6175.1508518309174</v>
+        <v>7934.4090808749643</v>
       </c>
       <c r="C19">
         <v>971.73017779133215</v>
       </c>
       <c r="D19">
-        <v>1844.248950043728</v>
+        <v>1888.107444918026</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -667,13 +667,13 @@
         <v>0.6</v>
       </c>
       <c r="B20">
-        <v>6294.2548916873566</v>
+        <v>8091.6896000928291</v>
       </c>
       <c r="C20">
         <v>1123.4788715138361</v>
       </c>
       <c r="D20">
-        <v>1447.681058926584</v>
+        <v>1502.7110910298129</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -681,13 +681,13 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21">
-        <v>6325.5852298297459</v>
+        <v>8128.6249263326026</v>
       </c>
       <c r="C21">
         <v>1136.154618253137</v>
       </c>
       <c r="D21">
-        <v>1298.0226871487159</v>
+        <v>1351.854507810848</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -695,13 +695,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B22">
-        <v>6373.8576158942433</v>
+        <v>8249.5272012321475</v>
       </c>
       <c r="C22">
         <v>991.42278196958034</v>
       </c>
       <c r="D22">
-        <v>818.27048496202701</v>
+        <v>865.92133840142242</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -709,13 +709,13 @@
         <v>0.7</v>
       </c>
       <c r="B23">
-        <v>6411.8002351206187</v>
+        <v>8271.349737002558</v>
       </c>
       <c r="C23">
         <v>1132.793556082125</v>
       </c>
       <c r="D23">
-        <v>553.25060151157879</v>
+        <v>594.50865899265602</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -723,13 +723,13 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="B24">
-        <v>6418.7487202940101</v>
+        <v>8283.3270439147764</v>
       </c>
       <c r="C24">
         <v>1134.863180046259</v>
       </c>
       <c r="D24">
-        <v>541.2440766017279</v>
+        <v>444.95209229970538</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,13 +737,13 @@
         <v>0.76666666666666661</v>
       </c>
       <c r="B25">
-        <v>6381.3362259522164</v>
+        <v>8324.5893621095711</v>
       </c>
       <c r="C25">
         <v>1142.7758874550959</v>
       </c>
       <c r="D25">
-        <v>115.1356865679351</v>
+        <v>103.010632640355</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -751,13 +751,13 @@
         <v>0.8</v>
       </c>
       <c r="B26">
-        <v>6381.7210744278127</v>
+        <v>8321.1841228069097</v>
       </c>
       <c r="C26">
         <v>1142.7758874550959</v>
       </c>
       <c r="D26">
-        <v>115.1356849351305</v>
+        <v>103.0106324305509</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,13 +765,13 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B27">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C27">
         <v>1142.7758874550959</v>
       </c>
       <c r="D27">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,13 +779,13 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C28">
         <v>1142.7758874550959</v>
       </c>
       <c r="D28">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -793,13 +793,13 @@
         <v>0.9</v>
       </c>
       <c r="B29">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C29">
         <v>1142.7758874550959</v>
       </c>
       <c r="D29">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,13 +807,13 @@
         <v>0.93333333333333335</v>
       </c>
       <c r="B30">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C30">
         <v>1142.7758874550959</v>
       </c>
       <c r="D30">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -821,13 +821,13 @@
         <v>0.96666666666666667</v>
       </c>
       <c r="B31">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C31">
         <v>1142.7758874550959</v>
       </c>
       <c r="D31">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -835,13 +835,13 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C32">
         <v>1142.7758874550959</v>
       </c>
       <c r="D32">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,13 +849,13 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C33">
         <v>1142.7758874550959</v>
       </c>
       <c r="D33">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -863,13 +863,13 @@
         <v>1.0666666666666671</v>
       </c>
       <c r="B34">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C34">
         <v>1142.7758874550959</v>
       </c>
       <c r="D34">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -877,13 +877,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B35">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C35">
         <v>1142.7758874550959</v>
       </c>
       <c r="D35">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -891,13 +891,13 @@
         <v>1.1333333333333331</v>
       </c>
       <c r="B36">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C36">
         <v>1142.7758874550959</v>
       </c>
       <c r="D36">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,13 +905,13 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C37">
         <v>1142.7758874550959</v>
       </c>
       <c r="D37">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -919,13 +919,13 @@
         <v>1.2</v>
       </c>
       <c r="B38">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C38">
         <v>1142.7758874550959</v>
       </c>
       <c r="D38">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -933,13 +933,13 @@
         <v>1.2333333333333329</v>
       </c>
       <c r="B39">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C39">
         <v>1142.7758874550959</v>
       </c>
       <c r="D39">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,13 +947,13 @@
         <v>1.2666666666666671</v>
       </c>
       <c r="B40">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C40">
         <v>1142.7758874550959</v>
       </c>
       <c r="D40">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,13 +961,13 @@
         <v>1.3</v>
       </c>
       <c r="B41">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C41">
         <v>1142.7758874550959</v>
       </c>
       <c r="D41">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,13 +975,13 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C42">
         <v>1142.7758874550959</v>
       </c>
       <c r="D42">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -989,13 +989,13 @@
         <v>1.3666666666666669</v>
       </c>
       <c r="B43">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C43">
         <v>1142.7758874550959</v>
       </c>
       <c r="D43">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,13 +1003,13 @@
         <v>1.4</v>
       </c>
       <c r="B44">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C44">
         <v>1142.7758874550959</v>
       </c>
       <c r="D44">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,13 +1017,13 @@
         <v>1.4333333333333329</v>
       </c>
       <c r="B45">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C45">
         <v>1142.7758874550959</v>
       </c>
       <c r="D45">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1031,13 +1031,13 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C46">
         <v>1142.7758874550959</v>
       </c>
       <c r="D46">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1045,13 +1045,13 @@
         <v>1.5</v>
       </c>
       <c r="B47">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C47">
         <v>1142.7758874550959</v>
       </c>
       <c r="D47">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,13 +1059,13 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C48">
         <v>1142.7758874550959</v>
       </c>
       <c r="D48">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1073,13 +1073,13 @@
         <v>1.5666666666666671</v>
       </c>
       <c r="B49">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C49">
         <v>1142.7758874550959</v>
       </c>
       <c r="D49">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1087,13 +1087,13 @@
         <v>1.6</v>
       </c>
       <c r="B50">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C50">
         <v>1142.7758874550959</v>
       </c>
       <c r="D50">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1101,13 +1101,13 @@
         <v>1.6333333333333331</v>
       </c>
       <c r="B51">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C51">
         <v>1142.7758874550959</v>
       </c>
       <c r="D51">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1115,13 +1115,13 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C52">
         <v>1142.7758874550959</v>
       </c>
       <c r="D52">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1129,13 +1129,13 @@
         <v>1.7</v>
       </c>
       <c r="B53">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C53">
         <v>1142.7758874550959</v>
       </c>
       <c r="D53">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1143,13 +1143,13 @@
         <v>1.7333333333333329</v>
       </c>
       <c r="B54">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C54">
         <v>1142.7758874550959</v>
       </c>
       <c r="D54">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,13 +1157,13 @@
         <v>1.7666666666666671</v>
       </c>
       <c r="B55">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C55">
         <v>1142.7758874550959</v>
       </c>
       <c r="D55">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1171,13 +1171,13 @@
         <v>1.8</v>
       </c>
       <c r="B56">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C56">
         <v>1142.7758874550959</v>
       </c>
       <c r="D56">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1185,13 +1185,13 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C57">
         <v>1142.7758874550959</v>
       </c>
       <c r="D57">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1199,13 +1199,13 @@
         <v>1.8666666666666669</v>
       </c>
       <c r="B58">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C58">
         <v>1142.7758874550959</v>
       </c>
       <c r="D58">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,13 +1213,13 @@
         <v>1.9</v>
       </c>
       <c r="B59">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C59">
         <v>1142.7758874550959</v>
       </c>
       <c r="D59">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,13 +1227,13 @@
         <v>1.9333333333333329</v>
       </c>
       <c r="B60">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C60">
         <v>1142.7758874550959</v>
       </c>
       <c r="D60">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,13 +1241,13 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C61">
         <v>1142.7758874550959</v>
       </c>
       <c r="D61">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,13 +1255,13 @@
         <v>2</v>
       </c>
       <c r="B62">
-        <v>6381.7754337876813</v>
+        <v>8321.2929399939439</v>
       </c>
       <c r="C62">
         <v>1142.7758874550959</v>
       </c>
       <c r="D62">
-        <v>115.1356839686669</v>
+        <v>103.0106324113675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>